<commit_message>
added unit multiplier in values, changed to assign UNPD and NET MIGRATION there
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v6.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/TransMonEE/data-etl/tmee/data_in/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="13_ncr:1_{0D7C4ACD-3B96-48F3-99D4-5E393553EB86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4965F45-C7E8-4BA3-80B4-29EC3215EA2A}"/>
+  <xr:revisionPtr revIDLastSave="281" documentId="13_ncr:1_{0D7C4ACD-3B96-48F3-99D4-5E393553EB86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9A305720-AB5E-41F6-9CA8-5C5BE95DCA65}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6034" uniqueCount="3020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6041" uniqueCount="3022">
   <si>
     <t>snapshot_id</t>
   </si>
@@ -8800,9 +8800,6 @@
     <t>Total population by age (expressed in thousands)</t>
   </si>
   <si>
-    <t>Customized for UNPD population. Not sure if ALL observations are estimated (e.g. OBS_STATUS in Helix are either PR:projections or not specified). Further research: UNPD references about methods and frequency of collection.</t>
-  </si>
-  <si>
     <t>HT_DIST79DTP3_P</t>
   </si>
   <si>
@@ -9104,6 +9101,15 @@
   </si>
   <si>
     <t>Proportion of poor population receiving social assistance cash benefit (%)</t>
+  </si>
+  <si>
+    <t>Unit_Mult</t>
+  </si>
+  <si>
+    <t>Expressed in thousands. Customized for UNPD population. Not sure if ALL observations are estimated (e.g. OBS_STATUS in Helix are either PR:projections or not specified). Further research: UNPD references about methods and frequency of collection.</t>
+  </si>
+  <si>
+    <t>Expressed in thousands. Customized for Net Migration (UNPD taken from WB collection)</t>
   </si>
 </sst>
 </file>
@@ -9859,8 +9865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L237"/>
   <sheetViews>
-    <sheetView topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="F226" sqref="F226"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9939,7 +9945,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f>VLOOKUP(F2,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F2,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -9974,7 +9980,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f>VLOOKUP(F3,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F3,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -10009,7 +10015,7 @@
         <v>562</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f>VLOOKUP(F4,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F4,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -10041,10 +10047,10 @@
         <v>2021</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>565</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>VLOOKUP(F5,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F5,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -10079,7 +10085,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f>VLOOKUP(F6,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F6,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>RATE_100</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -10114,7 +10120,7 @@
         <v>18</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f>VLOOKUP(F7,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F7,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -10149,7 +10155,7 @@
         <v>23</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f>VLOOKUP(F8,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F8,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>RATE_1000</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -10184,7 +10190,7 @@
         <v>18</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f>VLOOKUP(F9,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F9,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -10218,7 +10224,7 @@
         <v>68</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f>VLOOKUP(F10,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F10,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>RATE_1000</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -10252,7 +10258,7 @@
         <v>87</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f>VLOOKUP(F11,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F11,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>YR</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -10286,7 +10292,7 @@
         <v>44</v>
       </c>
       <c r="G12" s="25" t="str">
-        <f>VLOOKUP(F12,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F12,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>D_PER_1000_B</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -10320,7 +10326,7 @@
         <v>44</v>
       </c>
       <c r="G13" s="25" t="str">
-        <f>VLOOKUP(F13,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F13,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>D_PER_1000_B</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -10354,7 +10360,7 @@
         <v>27</v>
       </c>
       <c r="G14" s="25" t="str">
-        <f>VLOOKUP(F14,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F14,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>D_PER_1000_B</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -10388,7 +10394,7 @@
         <v>517</v>
       </c>
       <c r="G15" s="25" t="str">
-        <f>VLOOKUP(F15,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F15,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PER100KLIVEBIRTHS</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -10422,7 +10428,7 @@
         <v>563</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>VLOOKUP(F16,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F16,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>RATE_100000</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -10456,7 +10462,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>VLOOKUP(F17,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F17,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -10490,7 +10496,7 @@
         <v>540</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>VLOOKUP(F18,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F18,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>RATE_100000</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -10524,7 +10530,7 @@
         <v>541</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>VLOOKUP(F19,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F19,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>RATE_1000</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -10558,7 +10564,7 @@
         <v>542</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>VLOOKUP(F20,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F20,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -10592,7 +10598,7 @@
         <v>543</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>VLOOKUP(F21,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F21,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -10626,7 +10632,7 @@
         <v>18</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>VLOOKUP(F22,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F22,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -10660,7 +10666,7 @@
         <v>18</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>VLOOKUP(F23,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F23,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -10694,7 +10700,7 @@
         <v>18</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>VLOOKUP(F24,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F24,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -10728,7 +10734,7 @@
         <v>543</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>VLOOKUP(F25,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F25,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -10762,7 +10768,7 @@
         <v>543</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>VLOOKUP(F26,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F26,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -10796,7 +10802,7 @@
         <v>544</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>VLOOKUP(F27,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F27,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -10830,7 +10836,7 @@
         <v>18</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>VLOOKUP(F28,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F28,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -10864,7 +10870,7 @@
         <v>18</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>VLOOKUP(F29,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F29,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -10898,7 +10904,7 @@
         <v>18</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>VLOOKUP(F30,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F30,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -10932,7 +10938,7 @@
         <v>545</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>VLOOKUP(F31,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F31,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -10966,7 +10972,7 @@
         <v>18</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>VLOOKUP(F32,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F32,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -11000,7 +11006,7 @@
         <v>546</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>VLOOKUP(F33,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F33,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GPERM3</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -11034,7 +11040,7 @@
         <v>544</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>VLOOKUP(F34,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F34,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -11068,7 +11074,7 @@
         <v>547</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>VLOOKUP(F35,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F35,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -11102,7 +11108,7 @@
         <v>547</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>VLOOKUP(F36,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F36,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -11136,7 +11142,7 @@
         <v>547</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>VLOOKUP(F37,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F37,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -11170,7 +11176,7 @@
         <v>547</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>VLOOKUP(F38,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F38,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -11204,7 +11210,7 @@
         <v>547</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>VLOOKUP(F39,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F39,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -11238,7 +11244,7 @@
         <v>18</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>VLOOKUP(F40,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F40,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -11272,7 +11278,7 @@
         <v>548</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>VLOOKUP(F41,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F41,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -11306,7 +11312,7 @@
         <v>548</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>VLOOKUP(F42,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F42,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -11340,7 +11346,7 @@
         <v>548</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>VLOOKUP(F43,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F43,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H43" s="1" t="s">
@@ -11374,7 +11380,7 @@
         <v>542</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>VLOOKUP(F44,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F44,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H44" s="1" t="s">
@@ -11408,7 +11414,7 @@
         <v>87</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>VLOOKUP(F45,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F45,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>YR</v>
       </c>
       <c r="H45" s="1" t="s">
@@ -11442,7 +11448,7 @@
         <v>87</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>VLOOKUP(F46,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F46,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>YR</v>
       </c>
       <c r="H46" s="1" t="s">
@@ -11476,7 +11482,7 @@
         <v>548</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>VLOOKUP(F47,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F47,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H47" s="1" t="s">
@@ -11510,7 +11516,7 @@
         <v>548</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>VLOOKUP(F48,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F48,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H48" s="1" t="s">
@@ -11544,7 +11550,7 @@
         <v>548</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>VLOOKUP(F49,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F49,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H49" s="1" t="s">
@@ -11578,7 +11584,7 @@
         <v>542</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>VLOOKUP(F50,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F50,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H50" s="1" t="s">
@@ -11612,7 +11618,7 @@
         <v>542</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>VLOOKUP(F51,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F51,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H51" s="1" t="s">
@@ -11646,7 +11652,7 @@
         <v>18</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>VLOOKUP(F52,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F52,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H52" s="1" t="s">
@@ -11680,7 +11686,7 @@
         <v>18</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>VLOOKUP(F53,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F53,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -11714,7 +11720,7 @@
         <v>542</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>VLOOKUP(F54,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F54,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -11748,7 +11754,7 @@
         <v>544</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>VLOOKUP(F55,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F55,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H55" s="1" t="s">
@@ -11782,7 +11788,7 @@
         <v>544</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>VLOOKUP(F56,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F56,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H56" s="1" t="s">
@@ -11816,7 +11822,7 @@
         <v>542</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f>VLOOKUP(F57,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F57,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H57" s="1" t="s">
@@ -11850,7 +11856,7 @@
         <v>548</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f>VLOOKUP(F58,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F58,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H58" s="1" t="s">
@@ -11884,7 +11890,7 @@
         <v>18</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f>VLOOKUP(F59,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F59,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H59" s="1" t="s">
@@ -11918,7 +11924,7 @@
         <v>548</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f>VLOOKUP(F60,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F60,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H60" s="1" t="s">
@@ -11952,7 +11958,7 @@
         <v>18</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f>VLOOKUP(F61,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F61,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H61" s="1" t="s">
@@ -11986,7 +11992,7 @@
         <v>548</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f>VLOOKUP(F62,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F62,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H62" s="1" t="s">
@@ -12020,7 +12026,7 @@
         <v>18</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f>VLOOKUP(F63,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F63,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H63" s="1" t="s">
@@ -12054,7 +12060,7 @@
         <v>18</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f>VLOOKUP(F64,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F64,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H64" s="1" t="s">
@@ -12088,7 +12094,7 @@
         <v>18</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f>VLOOKUP(F65,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F65,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H65" s="1" t="s">
@@ -12122,7 +12128,7 @@
         <v>548</v>
       </c>
       <c r="G66" s="1" t="str">
-        <f>VLOOKUP(F66,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F66,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H66" s="1" t="s">
@@ -12156,7 +12162,7 @@
         <v>548</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f>VLOOKUP(F67,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F67,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H67" s="1" t="s">
@@ -12190,7 +12196,7 @@
         <v>548</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f>VLOOKUP(F68,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F68,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H68" s="1" t="s">
@@ -12224,7 +12230,7 @@
         <v>548</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f>VLOOKUP(F69,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F69,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H69" s="1" t="s">
@@ -12258,7 +12264,7 @@
         <v>18</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f>VLOOKUP(F70,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F70,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H70" s="1" t="s">
@@ -12292,7 +12298,7 @@
         <v>548</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f>VLOOKUP(F71,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F71,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H71" s="1" t="s">
@@ -12326,7 +12332,7 @@
         <v>548</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f>VLOOKUP(F72,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F72,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H72" s="1" t="s">
@@ -12360,7 +12366,7 @@
         <v>18</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f>VLOOKUP(F73,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F73,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H73" s="1" t="s">
@@ -12394,7 +12400,7 @@
         <v>548</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f>VLOOKUP(F74,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F74,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H74" s="1" t="s">
@@ -12428,7 +12434,7 @@
         <v>548</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f>VLOOKUP(F75,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F75,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H75" s="1" t="s">
@@ -12462,7 +12468,7 @@
         <v>18</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f>VLOOKUP(F76,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F76,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H76" s="1" t="s">
@@ -12496,7 +12502,7 @@
         <v>548</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f>VLOOKUP(F77,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F77,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H77" s="1" t="s">
@@ -12530,7 +12536,7 @@
         <v>548</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f>VLOOKUP(F78,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F78,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H78" s="1" t="s">
@@ -12564,7 +12570,7 @@
         <v>548</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f>VLOOKUP(F79,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F79,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H79" s="1" t="s">
@@ -12598,7 +12604,7 @@
         <v>548</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f>VLOOKUP(F80,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F80,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H80" s="1" t="s">
@@ -12632,7 +12638,7 @@
         <v>549</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f>VLOOKUP(F81,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F81,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H81" s="1" t="s">
@@ -12666,7 +12672,7 @@
         <v>542</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f>VLOOKUP(F82,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F82,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H82" s="1" t="s">
@@ -12700,7 +12706,7 @@
         <v>542</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f>VLOOKUP(F83,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F83,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H83" s="1" t="s">
@@ -12734,7 +12740,7 @@
         <v>542</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f>VLOOKUP(F84,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F84,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H84" s="1" t="s">
@@ -12768,7 +12774,7 @@
         <v>542</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f>VLOOKUP(F85,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F85,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H85" s="1" t="s">
@@ -12802,7 +12808,7 @@
         <v>542</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f>VLOOKUP(F86,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F86,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H86" s="1" t="s">
@@ -12836,7 +12842,7 @@
         <v>542</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f>VLOOKUP(F87,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F87,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H87" s="1" t="s">
@@ -12870,7 +12876,7 @@
         <v>542</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f>VLOOKUP(F88,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F88,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H88" s="1" t="s">
@@ -12904,7 +12910,7 @@
         <v>542</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f>VLOOKUP(F89,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F89,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H89" s="1" t="s">
@@ -12938,7 +12944,7 @@
         <v>542</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f>VLOOKUP(F90,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F90,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H90" s="1" t="s">
@@ -12972,7 +12978,7 @@
         <v>550</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f>VLOOKUP(F91,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F91,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H91" s="1" t="s">
@@ -13006,7 +13012,7 @@
         <v>550</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f>VLOOKUP(F92,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F92,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H92" s="1" t="s">
@@ -13040,7 +13046,7 @@
         <v>550</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f>VLOOKUP(F93,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F93,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H93" s="1" t="s">
@@ -13074,7 +13080,7 @@
         <v>550</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f>VLOOKUP(F94,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F94,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H94" s="1" t="s">
@@ -13108,7 +13114,7 @@
         <v>550</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f>VLOOKUP(F95,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F95,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H95" s="1" t="s">
@@ -13142,7 +13148,7 @@
         <v>550</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f>VLOOKUP(F96,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F96,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H96" s="1" t="s">
@@ -13176,7 +13182,7 @@
         <v>551</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f>VLOOKUP(F97,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F97,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>NUMBER</v>
       </c>
       <c r="H97" s="1" t="s">
@@ -13210,7 +13216,7 @@
         <v>551</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f>VLOOKUP(F98,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F98,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>NUMBER</v>
       </c>
       <c r="H98" s="1" t="s">
@@ -13244,7 +13250,7 @@
         <v>551</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f>VLOOKUP(F99,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F99,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>NUMBER</v>
       </c>
       <c r="H99" s="1" t="s">
@@ -13278,7 +13284,7 @@
         <v>551</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f>VLOOKUP(F100,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F100,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>NUMBER</v>
       </c>
       <c r="H100" s="1" t="s">
@@ -13312,7 +13318,7 @@
         <v>552</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f>VLOOKUP(F101,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F101,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>SCORE</v>
       </c>
       <c r="H101" s="1" t="s">
@@ -13346,7 +13352,7 @@
         <v>552</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f>VLOOKUP(F102,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F102,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>SCORE</v>
       </c>
       <c r="H102" s="1" t="s">
@@ -13380,7 +13386,7 @@
         <v>552</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f>VLOOKUP(F103,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F103,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>SCORE</v>
       </c>
       <c r="H103" s="1" t="s">
@@ -13414,7 +13420,7 @@
         <v>552</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f>VLOOKUP(F104,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F104,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>SCORE</v>
       </c>
       <c r="H104" s="1" t="s">
@@ -13448,7 +13454,7 @@
         <v>553</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f>VLOOKUP(F105,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F105,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>SCORE</v>
       </c>
       <c r="H105" s="1" t="s">
@@ -13482,7 +13488,7 @@
         <v>554</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f>VLOOKUP(F106,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F106,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>SCORE</v>
       </c>
       <c r="H106" s="1" t="s">
@@ -13516,7 +13522,7 @@
         <v>554</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f>VLOOKUP(F107,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F107,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>SCORE</v>
       </c>
       <c r="H107" s="1" t="s">
@@ -13550,7 +13556,7 @@
         <v>554</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f>VLOOKUP(F108,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F108,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>SCORE</v>
       </c>
       <c r="H108" s="1" t="s">
@@ -13584,7 +13590,7 @@
         <v>542</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f>VLOOKUP(F109,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F109,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H109" s="1" t="s">
@@ -13618,7 +13624,7 @@
         <v>548</v>
       </c>
       <c r="G110" s="1" t="str">
-        <f>VLOOKUP(F110,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F110,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H110" s="1" t="s">
@@ -13652,7 +13658,7 @@
         <v>548</v>
       </c>
       <c r="G111" s="1" t="str">
-        <f>VLOOKUP(F111,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F111,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H111" s="1" t="s">
@@ -13686,7 +13692,7 @@
         <v>542</v>
       </c>
       <c r="G112" s="1" t="str">
-        <f>VLOOKUP(F112,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F112,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H112" s="1" t="s">
@@ -13720,7 +13726,7 @@
         <v>542</v>
       </c>
       <c r="G113" s="1" t="str">
-        <f>VLOOKUP(F113,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F113,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H113" s="1" t="s">
@@ -13754,7 +13760,7 @@
         <v>18</v>
       </c>
       <c r="G114" s="1" t="str">
-        <f>VLOOKUP(F114,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F114,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H114" s="1" t="s">
@@ -13788,7 +13794,7 @@
         <v>542</v>
       </c>
       <c r="G115" s="1" t="str">
-        <f>VLOOKUP(F115,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F115,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H115" s="1" t="s">
@@ -13822,7 +13828,7 @@
         <v>548</v>
       </c>
       <c r="G116" s="1" t="str">
-        <f>VLOOKUP(F116,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F116,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H116" s="1" t="s">
@@ -13856,7 +13862,7 @@
         <v>542</v>
       </c>
       <c r="G117" s="1" t="str">
-        <f>VLOOKUP(F117,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F117,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H117" s="1" t="s">
@@ -13890,7 +13896,7 @@
         <v>542</v>
       </c>
       <c r="G118" s="1" t="str">
-        <f>VLOOKUP(F118,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F118,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H118" s="1" t="s">
@@ -13924,7 +13930,7 @@
         <v>542</v>
       </c>
       <c r="G119" s="1" t="str">
-        <f>VLOOKUP(F119,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F119,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H119" s="1" t="s">
@@ -13958,7 +13964,7 @@
         <v>544</v>
       </c>
       <c r="G120" s="1" t="str">
-        <f>VLOOKUP(F120,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F120,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H120" s="1" t="s">
@@ -13992,7 +13998,7 @@
         <v>544</v>
       </c>
       <c r="G121" s="1" t="str">
-        <f>VLOOKUP(F121,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F121,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H121" s="1" t="s">
@@ -14026,7 +14032,7 @@
         <v>544</v>
       </c>
       <c r="G122" s="1" t="str">
-        <f>VLOOKUP(F122,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F122,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H122" s="1" t="s">
@@ -14060,7 +14066,7 @@
         <v>542</v>
       </c>
       <c r="G123" s="1" t="str">
-        <f>VLOOKUP(F123,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F123,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H123" s="1" t="s">
@@ -14094,7 +14100,7 @@
         <v>548</v>
       </c>
       <c r="G124" s="1" t="str">
-        <f>VLOOKUP(F124,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F124,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H124" s="1" t="s">
@@ -14128,7 +14134,7 @@
         <v>542</v>
       </c>
       <c r="G125" s="1" t="str">
-        <f>VLOOKUP(F125,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F125,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H125" s="1" t="s">
@@ -14162,7 +14168,7 @@
         <v>548</v>
       </c>
       <c r="G126" s="1" t="str">
-        <f>VLOOKUP(F126,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F126,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H126" s="1" t="s">
@@ -14196,7 +14202,7 @@
         <v>542</v>
       </c>
       <c r="G127" s="1" t="str">
-        <f>VLOOKUP(F127,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F127,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H127" s="1" t="s">
@@ -14230,7 +14236,7 @@
         <v>548</v>
       </c>
       <c r="G128" s="1" t="str">
-        <f>VLOOKUP(F128,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F128,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H128" s="1" t="s">
@@ -14264,7 +14270,7 @@
         <v>542</v>
       </c>
       <c r="G129" s="1" t="str">
-        <f>VLOOKUP(F129,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F129,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H129" s="1" t="s">
@@ -14298,7 +14304,7 @@
         <v>542</v>
       </c>
       <c r="G130" s="1" t="str">
-        <f>VLOOKUP(F130,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F130,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H130" s="1" t="s">
@@ -14332,7 +14338,7 @@
         <v>542</v>
       </c>
       <c r="G131" s="1" t="str">
-        <f>VLOOKUP(F131,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F131,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H131" s="1" t="s">
@@ -14366,7 +14372,7 @@
         <v>548</v>
       </c>
       <c r="G132" s="1" t="str">
-        <f>VLOOKUP(F132,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F132,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H132" s="1" t="s">
@@ -14400,7 +14406,7 @@
         <v>548</v>
       </c>
       <c r="G133" s="1" t="str">
-        <f>VLOOKUP(F133,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F133,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H133" s="1" t="s">
@@ -14434,7 +14440,7 @@
         <v>548</v>
       </c>
       <c r="G134" s="1" t="str">
-        <f>VLOOKUP(F134,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F134,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H134" s="1" t="s">
@@ -14468,7 +14474,7 @@
         <v>18</v>
       </c>
       <c r="G135" s="1" t="str">
-        <f>VLOOKUP(F135,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F135,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H135" s="1" t="s">
@@ -14502,7 +14508,7 @@
         <v>18</v>
       </c>
       <c r="G136" s="1" t="str">
-        <f>VLOOKUP(F136,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F136,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H136" s="1" t="s">
@@ -14536,7 +14542,7 @@
         <v>548</v>
       </c>
       <c r="G137" s="1" t="str">
-        <f>VLOOKUP(F137,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F137,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H137" s="1" t="s">
@@ -14570,7 +14576,7 @@
         <v>548</v>
       </c>
       <c r="G138" s="1" t="str">
-        <f>VLOOKUP(F138,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F138,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H138" s="1" t="s">
@@ -14604,7 +14610,7 @@
         <v>548</v>
       </c>
       <c r="G139" s="1" t="str">
-        <f>VLOOKUP(F139,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F139,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H139" s="1" t="s">
@@ -14638,7 +14644,7 @@
         <v>18</v>
       </c>
       <c r="G140" s="1" t="str">
-        <f>VLOOKUP(F140,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F140,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H140" s="1" t="s">
@@ -14672,7 +14678,7 @@
         <v>18</v>
       </c>
       <c r="G141" s="1" t="str">
-        <f>VLOOKUP(F141,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F141,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H141" s="1" t="s">
@@ -14706,7 +14712,7 @@
         <v>555</v>
       </c>
       <c r="G142" s="1" t="str">
-        <f>VLOOKUP(F142,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F142,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GPI</v>
       </c>
       <c r="H142" s="1" t="s">
@@ -14740,7 +14746,7 @@
         <v>555</v>
       </c>
       <c r="G143" s="1" t="str">
-        <f>VLOOKUP(F143,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F143,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GPI</v>
       </c>
       <c r="H143" s="1" t="s">
@@ -14774,7 +14780,7 @@
         <v>555</v>
       </c>
       <c r="G144" s="1" t="str">
-        <f>VLOOKUP(F144,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F144,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GPI</v>
       </c>
       <c r="H144" s="1" t="s">
@@ -14808,7 +14814,7 @@
         <v>555</v>
       </c>
       <c r="G145" s="1" t="str">
-        <f>VLOOKUP(F145,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F145,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GPI</v>
       </c>
       <c r="H145" s="1" t="s">
@@ -14842,7 +14848,7 @@
         <v>555</v>
       </c>
       <c r="G146" s="1" t="str">
-        <f>VLOOKUP(F146,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F146,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GPI</v>
       </c>
       <c r="H146" s="1" t="s">
@@ -14876,7 +14882,7 @@
         <v>556</v>
       </c>
       <c r="G147" s="1" t="str">
-        <f>VLOOKUP(F147,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F147,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GDP_PERC</v>
       </c>
       <c r="H147" s="1" t="s">
@@ -14910,7 +14916,7 @@
         <v>557</v>
       </c>
       <c r="G148" s="1" t="str">
-        <f>VLOOKUP(F148,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F148,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GOV_EXP_T</v>
       </c>
       <c r="H148" s="1" t="s">
@@ -14944,7 +14950,7 @@
         <v>558</v>
       </c>
       <c r="G149" s="1" t="str">
-        <f>VLOOKUP(F149,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F149,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PPP_CONST</v>
       </c>
       <c r="H149" s="1" t="s">
@@ -14978,7 +14984,7 @@
         <v>559</v>
       </c>
       <c r="G150" s="1" t="str">
-        <f>VLOOKUP(F150,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F150,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GOV_EXP_EDU</v>
       </c>
       <c r="H150" s="1" t="s">
@@ -15012,7 +15018,7 @@
         <v>559</v>
       </c>
       <c r="G151" s="1" t="str">
-        <f>VLOOKUP(F151,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F151,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GOV_EXP_EDU</v>
       </c>
       <c r="H151" s="1" t="s">
@@ -15046,7 +15052,7 @@
         <v>559</v>
       </c>
       <c r="G152" s="1" t="str">
-        <f>VLOOKUP(F152,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F152,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GOV_EXP_EDU</v>
       </c>
       <c r="H152" s="1" t="s">
@@ -15080,7 +15086,7 @@
         <v>559</v>
       </c>
       <c r="G153" s="1" t="str">
-        <f>VLOOKUP(F153,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F153,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GOV_EXP_EDU</v>
       </c>
       <c r="H153" s="1" t="s">
@@ -15114,7 +15120,7 @@
         <v>559</v>
       </c>
       <c r="G154" s="1" t="str">
-        <f>VLOOKUP(F154,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F154,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GOV_EXP_EDU</v>
       </c>
       <c r="H154" s="1" t="s">
@@ -15148,7 +15154,7 @@
         <v>559</v>
       </c>
       <c r="G155" s="1" t="str">
-        <f>VLOOKUP(F155,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F155,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GOV_EXP_EDU</v>
       </c>
       <c r="H155" s="1" t="s">
@@ -15182,7 +15188,7 @@
         <v>18</v>
       </c>
       <c r="G156" s="1" t="str">
-        <f>VLOOKUP(F156,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F156,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H156" s="1" t="s">
@@ -15216,7 +15222,7 @@
         <v>18</v>
       </c>
       <c r="G157" s="1" t="str">
-        <f>VLOOKUP(F157,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F157,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H157" s="1" t="s">
@@ -15250,7 +15256,7 @@
         <v>18</v>
       </c>
       <c r="G158" s="1" t="str">
-        <f>VLOOKUP(F158,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F158,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H158" s="1" t="s">
@@ -15284,7 +15290,7 @@
         <v>560</v>
       </c>
       <c r="G159" s="1" t="str">
-        <f>VLOOKUP(F159,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F159,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H159" s="1" t="s">
@@ -15318,7 +15324,7 @@
         <v>560</v>
       </c>
       <c r="G160" s="1" t="str">
-        <f>VLOOKUP(F160,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F160,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H160" s="1" t="s">
@@ -15352,7 +15358,7 @@
         <v>560</v>
       </c>
       <c r="G161" s="1" t="str">
-        <f>VLOOKUP(F161,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F161,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H161" s="1" t="s">
@@ -15386,7 +15392,7 @@
         <v>548</v>
       </c>
       <c r="G162" s="1" t="str">
-        <f>VLOOKUP(F162,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F162,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H162" s="1" t="s">
@@ -15420,7 +15426,7 @@
         <v>548</v>
       </c>
       <c r="G163" s="1" t="str">
-        <f>VLOOKUP(F163,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F163,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H163" s="1" t="s">
@@ -15454,7 +15460,7 @@
         <v>548</v>
       </c>
       <c r="G164" s="1" t="str">
-        <f>VLOOKUP(F164,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F164,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H164" s="1" t="s">
@@ -15488,7 +15494,7 @@
         <v>14</v>
       </c>
       <c r="G165" s="1" t="str">
-        <f>VLOOKUP(F165,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F165,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H165" s="1" t="s">
@@ -15522,7 +15528,7 @@
         <v>14</v>
       </c>
       <c r="G166" s="1" t="str">
-        <f>VLOOKUP(F166,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F166,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H166" s="1" t="s">
@@ -15556,7 +15562,7 @@
         <v>14</v>
       </c>
       <c r="G167" s="1" t="str">
-        <f>VLOOKUP(F167,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F167,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H167" s="1" t="s">
@@ -15590,7 +15596,7 @@
         <v>14</v>
       </c>
       <c r="G168" s="1" t="str">
-        <f>VLOOKUP(F168,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F168,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H168" s="1" t="s">
@@ -15624,7 +15630,7 @@
         <v>542</v>
       </c>
       <c r="G169" s="1" t="str">
-        <f>VLOOKUP(F169,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F169,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H169" s="1" t="s">
@@ -15658,7 +15664,7 @@
         <v>542</v>
       </c>
       <c r="G170" s="1" t="str">
-        <f>VLOOKUP(F170,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F170,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H170" s="1" t="s">
@@ -15692,7 +15698,7 @@
         <v>542</v>
       </c>
       <c r="G171" s="1" t="str">
-        <f>VLOOKUP(F171,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F171,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H171" s="1" t="s">
@@ -15726,7 +15732,7 @@
         <v>542</v>
       </c>
       <c r="G172" s="1" t="str">
-        <f>VLOOKUP(F172,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F172,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H172" s="1" t="s">
@@ -15760,7 +15766,7 @@
         <v>14</v>
       </c>
       <c r="G173" s="1" t="str">
-        <f>VLOOKUP(F173,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F173,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H173" s="1" t="s">
@@ -15794,7 +15800,7 @@
         <v>14</v>
       </c>
       <c r="G174" s="1" t="str">
-        <f>VLOOKUP(F174,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F174,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H174" s="1" t="s">
@@ -15828,7 +15834,7 @@
         <v>14</v>
       </c>
       <c r="G175" s="1" t="str">
-        <f>VLOOKUP(F175,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F175,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H175" s="1" t="s">
@@ -15862,7 +15868,7 @@
         <v>14</v>
       </c>
       <c r="G176" s="1" t="str">
-        <f>VLOOKUP(F176,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F176,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H176" s="1" t="s">
@@ -15896,7 +15902,7 @@
         <v>542</v>
       </c>
       <c r="G177" s="1" t="str">
-        <f>VLOOKUP(F177,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F177,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H177" s="1" t="s">
@@ -15930,7 +15936,7 @@
         <v>542</v>
       </c>
       <c r="G178" s="1" t="str">
-        <f>VLOOKUP(F178,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F178,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H178" s="1" t="s">
@@ -15964,7 +15970,7 @@
         <v>542</v>
       </c>
       <c r="G179" s="1" t="str">
-        <f>VLOOKUP(F179,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F179,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H179" s="1" t="s">
@@ -15998,7 +16004,7 @@
         <v>542</v>
       </c>
       <c r="G180" s="1" t="str">
-        <f>VLOOKUP(F180,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F180,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H180" s="1" t="s">
@@ -16032,7 +16038,7 @@
         <v>14</v>
       </c>
       <c r="G181" s="1" t="str">
-        <f>VLOOKUP(F181,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F181,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H181" s="1" t="s">
@@ -16066,7 +16072,7 @@
         <v>14</v>
       </c>
       <c r="G182" s="1" t="str">
-        <f>VLOOKUP(F182,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F182,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H182" s="1" t="s">
@@ -16100,7 +16106,7 @@
         <v>14</v>
       </c>
       <c r="G183" s="1" t="str">
-        <f>VLOOKUP(F183,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F183,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H183" s="1" t="s">
@@ -16134,7 +16140,7 @@
         <v>14</v>
       </c>
       <c r="G184" s="1" t="str">
-        <f>VLOOKUP(F184,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F184,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H184" s="1" t="s">
@@ -16168,7 +16174,7 @@
         <v>547</v>
       </c>
       <c r="G185" s="1" t="str">
-        <f>VLOOKUP(F185,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F185,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H185" s="1" t="s">
@@ -16202,7 +16208,7 @@
         <v>544</v>
       </c>
       <c r="G186" s="1" t="str">
-        <f>VLOOKUP(F186,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F186,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H186" s="1" t="s">
@@ -16236,7 +16242,7 @@
         <v>542</v>
       </c>
       <c r="G187" s="1" t="str">
-        <f>VLOOKUP(F187,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F187,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H187" s="1" t="s">
@@ -16270,7 +16276,7 @@
         <v>551</v>
       </c>
       <c r="G188" s="1" t="str">
-        <f>VLOOKUP(F188,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F188,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>NUMBER</v>
       </c>
       <c r="H188" s="1" t="s">
@@ -16304,7 +16310,7 @@
         <v>551</v>
       </c>
       <c r="G189" s="1" t="str">
-        <f>VLOOKUP(F189,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F189,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>NUMBER</v>
       </c>
       <c r="H189" s="1" t="s">
@@ -16338,7 +16344,7 @@
         <v>542</v>
       </c>
       <c r="G190" s="1" t="str">
-        <f>VLOOKUP(F190,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F190,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H190" s="1" t="s">
@@ -16372,7 +16378,7 @@
         <v>542</v>
       </c>
       <c r="G191" s="1" t="str">
-        <f>VLOOKUP(F191,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F191,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H191" s="1" t="s">
@@ -16406,7 +16412,7 @@
         <v>542</v>
       </c>
       <c r="G192" s="1" t="str">
-        <f>VLOOKUP(F192,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F192,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H192" s="1" t="s">
@@ -16440,7 +16446,7 @@
         <v>542</v>
       </c>
       <c r="G193" s="1" t="str">
-        <f>VLOOKUP(F193,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F193,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H193" s="1" t="s">
@@ -16474,7 +16480,7 @@
         <v>542</v>
       </c>
       <c r="G194" s="1" t="str">
-        <f>VLOOKUP(F194,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F194,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H194" s="1" t="s">
@@ -16508,7 +16514,7 @@
         <v>542</v>
       </c>
       <c r="G195" s="1" t="str">
-        <f>VLOOKUP(F195,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F195,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H195" s="1" t="s">
@@ -16542,7 +16548,7 @@
         <v>542</v>
       </c>
       <c r="G196" s="1" t="str">
-        <f>VLOOKUP(F196,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F196,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H196" s="1" t="s">
@@ -16576,7 +16582,7 @@
         <v>542</v>
       </c>
       <c r="G197" s="1" t="str">
-        <f>VLOOKUP(F197,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F197,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H197" s="1" t="s">
@@ -16610,7 +16616,7 @@
         <v>542</v>
       </c>
       <c r="G198" s="1" t="str">
-        <f>VLOOKUP(F198,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F198,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H198" s="1" t="s">
@@ -16644,7 +16650,7 @@
         <v>542</v>
       </c>
       <c r="G199" s="1" t="str">
-        <f>VLOOKUP(F199,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F199,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H199" s="1" t="s">
@@ -16678,7 +16684,7 @@
         <v>542</v>
       </c>
       <c r="G200" s="1" t="str">
-        <f>VLOOKUP(F200,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F200,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H200" s="1" t="s">
@@ -16712,7 +16718,7 @@
         <v>542</v>
       </c>
       <c r="G201" s="1" t="str">
-        <f>VLOOKUP(F201,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F201,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H201" s="1" t="s">
@@ -16746,7 +16752,7 @@
         <v>542</v>
       </c>
       <c r="G202" s="1" t="str">
-        <f>VLOOKUP(F202,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F202,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H202" s="1" t="s">
@@ -16780,7 +16786,7 @@
         <v>542</v>
       </c>
       <c r="G203" s="1" t="str">
-        <f>VLOOKUP(F203,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F203,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H203" s="1" t="s">
@@ -16814,7 +16820,7 @@
         <v>542</v>
       </c>
       <c r="G204" s="1" t="str">
-        <f>VLOOKUP(F204,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F204,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H204" s="1" t="s">
@@ -16848,7 +16854,7 @@
         <v>542</v>
       </c>
       <c r="G205" s="1" t="str">
-        <f>VLOOKUP(F205,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F205,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H205" s="1" t="s">
@@ -16882,7 +16888,7 @@
         <v>18</v>
       </c>
       <c r="G206" s="1" t="str">
-        <f>VLOOKUP(F206,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F206,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H206" s="1" t="s">
@@ -16916,7 +16922,7 @@
         <v>548</v>
       </c>
       <c r="G207" s="1" t="str">
-        <f>VLOOKUP(F207,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F207,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H207" s="1" t="s">
@@ -16950,7 +16956,7 @@
         <v>542</v>
       </c>
       <c r="G208" s="1" t="str">
-        <f>VLOOKUP(F208,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F208,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H208" s="1" t="s">
@@ -16984,7 +16990,7 @@
         <v>555</v>
       </c>
       <c r="G209" s="1" t="str">
-        <f>VLOOKUP(F209,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F209,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>GPI</v>
       </c>
       <c r="H209" s="1" t="s">
@@ -17018,7 +17024,7 @@
         <v>548</v>
       </c>
       <c r="G210" s="1" t="str">
-        <f>VLOOKUP(F210,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F210,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H210" s="1" t="s">
@@ -17052,7 +17058,7 @@
         <v>548</v>
       </c>
       <c r="G211" s="1" t="str">
-        <f>VLOOKUP(F211,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F211,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H211" s="1" t="s">
@@ -17086,7 +17092,7 @@
         <v>548</v>
       </c>
       <c r="G212" s="1" t="str">
-        <f>VLOOKUP(F212,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F212,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H212" s="1" t="s">
@@ -17120,7 +17126,7 @@
         <v>548</v>
       </c>
       <c r="G213" s="1" t="str">
-        <f>VLOOKUP(F213,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F213,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H213" s="1" t="s">
@@ -17154,7 +17160,7 @@
         <v>548</v>
       </c>
       <c r="G214" s="1" t="str">
-        <f>VLOOKUP(F214,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F214,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H214" s="1" t="s">
@@ -17188,7 +17194,7 @@
         <v>548</v>
       </c>
       <c r="G215" s="1" t="str">
-        <f>VLOOKUP(F215,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F215,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H215" s="1" t="s">
@@ -17222,7 +17228,7 @@
         <v>542</v>
       </c>
       <c r="G216" s="1" t="str">
-        <f>VLOOKUP(F216,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F216,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H216" s="1" t="s">
@@ -17256,7 +17262,7 @@
         <v>548</v>
       </c>
       <c r="G217" s="1" t="str">
-        <f>VLOOKUP(F217,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F217,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H217" s="1" t="s">
@@ -17290,7 +17296,7 @@
         <v>18</v>
       </c>
       <c r="G218" s="1" t="str">
-        <f>VLOOKUP(F218,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F218,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H218" s="1" t="s">
@@ -17324,7 +17330,7 @@
         <v>548</v>
       </c>
       <c r="G219" s="1" t="str">
-        <f>VLOOKUP(F219,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F219,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PS</v>
       </c>
       <c r="H219" s="1" t="s">
@@ -17358,7 +17364,7 @@
         <v>18</v>
       </c>
       <c r="G220" s="1" t="str">
-        <f>VLOOKUP(F220,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F220,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H220" s="1" t="s">
@@ -17392,7 +17398,7 @@
         <v>564</v>
       </c>
       <c r="G221" s="1" t="str">
-        <f>VLOOKUP(F221,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F221,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H221" s="1" t="s">
@@ -17426,7 +17432,7 @@
         <v>564</v>
       </c>
       <c r="G222" s="1" t="str">
-        <f>VLOOKUP(F222,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F222,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H222" s="1" t="s">
@@ -17460,7 +17466,7 @@
         <v>564</v>
       </c>
       <c r="G223" s="1" t="str">
-        <f>VLOOKUP(F223,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F223,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H223" s="1" t="s">
@@ -17474,7 +17480,7 @@
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="B224" s="16" t="s">
         <v>1341</v>
@@ -17494,7 +17500,7 @@
         <v>18</v>
       </c>
       <c r="G224" s="1" t="str">
-        <f>VLOOKUP(F224,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F224,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H224" s="1" t="s">
@@ -17508,7 +17514,7 @@
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
-        <v>2994</v>
+        <v>2993</v>
       </c>
       <c r="B225" s="16" t="s">
         <v>1343</v>
@@ -17528,7 +17534,7 @@
         <v>18</v>
       </c>
       <c r="G225" s="1" t="str">
-        <f>VLOOKUP(F225,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F225,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H225" s="1" t="s">
@@ -17542,7 +17548,7 @@
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>2995</v>
+        <v>2994</v>
       </c>
       <c r="B226" s="16" t="s">
         <v>1345</v>
@@ -17562,7 +17568,7 @@
         <v>542</v>
       </c>
       <c r="G226" s="1" t="str">
-        <f>VLOOKUP(F226,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F226,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H226" s="1" t="s">
@@ -17576,7 +17582,7 @@
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
-        <v>2996</v>
+        <v>2995</v>
       </c>
       <c r="B227" s="16" t="s">
         <v>1347</v>
@@ -17596,7 +17602,7 @@
         <v>18</v>
       </c>
       <c r="G227" s="1" t="str">
-        <f>VLOOKUP(F227,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F227,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H227" s="1" t="s">
@@ -17610,7 +17616,7 @@
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>2997</v>
+        <v>2996</v>
       </c>
       <c r="B228" s="16" t="s">
         <v>1349</v>
@@ -17630,11 +17636,11 @@
         <v>18</v>
       </c>
       <c r="G228" s="1" t="str">
-        <f>VLOOKUP(F228,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F228,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H228" s="1" t="s">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="I228" s="25" t="str">
         <f>VLOOKUP(H228,Source!$A$2:$G$238,3,FALSE)</f>
@@ -17644,7 +17650,7 @@
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
-        <v>2998</v>
+        <v>2997</v>
       </c>
       <c r="B229" s="16" t="s">
         <v>1351</v>
@@ -17664,11 +17670,11 @@
         <v>542</v>
       </c>
       <c r="G229" s="1" t="str">
-        <f>VLOOKUP(F229,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F229,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H229" s="1" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="I229" s="25" t="str">
         <f>VLOOKUP(H229,Source!$A$2:$G$238,3,FALSE)</f>
@@ -17678,7 +17684,7 @@
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
-        <v>2999</v>
+        <v>2998</v>
       </c>
       <c r="B230" s="16" t="s">
         <v>1353</v>
@@ -17698,11 +17704,11 @@
         <v>542</v>
       </c>
       <c r="G230" s="1" t="str">
-        <f>VLOOKUP(F230,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F230,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H230" s="1" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="I230" s="25" t="str">
         <f>VLOOKUP(H230,Source!$A$2:$G$238,3,FALSE)</f>
@@ -17712,7 +17718,7 @@
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
-        <v>3000</v>
+        <v>2999</v>
       </c>
       <c r="B231" s="16" t="s">
         <v>1355</v>
@@ -17732,11 +17738,11 @@
         <v>542</v>
       </c>
       <c r="G231" s="1" t="str">
-        <f>VLOOKUP(F231,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F231,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H231" s="1" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="I231" s="25" t="str">
         <f>VLOOKUP(H231,Source!$A$2:$G$238,3,FALSE)</f>
@@ -17746,7 +17752,7 @@
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="B233" s="16" t="s">
         <v>1458</v>
@@ -17766,11 +17772,11 @@
         <v>547</v>
       </c>
       <c r="G233" s="1" t="str">
-        <f>VLOOKUP(F233,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F233,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H233" s="1" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="I233" s="25" t="str">
         <f>VLOOKUP(H233,Source!$A$2:$G$250,3,FALSE)</f>
@@ -17779,7 +17785,7 @@
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="B234" s="16" t="s">
         <v>1460</v>
@@ -17799,11 +17805,11 @@
         <v>547</v>
       </c>
       <c r="G234" s="1" t="str">
-        <f>VLOOKUP(F234,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F234,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H234" s="1" t="s">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="I234" s="25" t="str">
         <f>VLOOKUP(H234,Source!$A$2:$G$250,3,FALSE)</f>
@@ -17812,7 +17818,7 @@
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="B235" s="16" t="s">
         <v>1464</v>
@@ -17832,11 +17838,11 @@
         <v>544</v>
       </c>
       <c r="G235" s="1" t="str">
-        <f>VLOOKUP(F235,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F235,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>PCNT</v>
       </c>
       <c r="H235" s="1" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="I235" s="25" t="str">
         <f>VLOOKUP(H235,Source!$A$2:$G$250,3,FALSE)</f>
@@ -17845,7 +17851,7 @@
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="B236" s="16" t="s">
         <v>1842</v>
@@ -17865,11 +17871,11 @@
         <v>561</v>
       </c>
       <c r="G236" s="1" t="str">
-        <f>VLOOKUP(F236,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F236,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>BINARY</v>
       </c>
       <c r="H236" s="1" t="s">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="I236" s="25" t="str">
         <f>VLOOKUP(H236,Source!$A$2:$G$250,3,FALSE)</f>
@@ -17878,7 +17884,7 @@
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
-        <v>3005</v>
+        <v>3004</v>
       </c>
       <c r="B237" s="16" t="s">
         <v>1844</v>
@@ -17898,11 +17904,11 @@
         <v>561</v>
       </c>
       <c r="G237" s="1" t="str">
-        <f>VLOOKUP(F237,Value_type!$A$2:$H$107,3,FALSE)</f>
+        <f>VLOOKUP(F237,Value_type!$A$2:$I$107,3,FALSE)</f>
         <v>BINARY</v>
       </c>
       <c r="H237" s="1" t="s">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="I237" s="25" t="str">
         <f>VLOOKUP(H237,Source!$A$2:$G$250,3,FALSE)</f>
@@ -18446,9 +18452,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M657"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E276" sqref="E276"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D275" sqref="D275:D286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18826,13 +18832,13 @@
         <v>962</v>
       </c>
       <c r="E14" s="33" t="s">
+        <v>2924</v>
+      </c>
+      <c r="F14" s="25" t="s">
         <v>2925</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="M14" s="36" t="s">
         <v>2926</v>
-      </c>
-      <c r="M14" s="36" t="s">
-        <v>2927</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -19828,7 +19834,7 @@
         <v>2770</v>
       </c>
       <c r="F62" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
@@ -19868,7 +19874,7 @@
         <v>1046</v>
       </c>
       <c r="F64" t="s">
-        <v>2920</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
@@ -24178,14 +24184,14 @@
       <c r="C275" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D275" s="56" t="s">
+      <c r="D275" s="55" t="s">
+        <v>2929</v>
+      </c>
+      <c r="E275" s="57" t="s">
+        <v>3014</v>
+      </c>
+      <c r="F275" t="s">
         <v>2930</v>
-      </c>
-      <c r="E275" s="57" t="s">
-        <v>3015</v>
-      </c>
-      <c r="F275" t="s">
-        <v>2931</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.35">
@@ -24198,14 +24204,14 @@
       <c r="C276" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D276" s="56" t="s">
-        <v>2930</v>
+      <c r="D276" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E276" s="57" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="F276" t="s">
-        <v>2933</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.35">
@@ -24218,14 +24224,14 @@
       <c r="C277" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D277" s="56" t="s">
-        <v>2930</v>
+      <c r="D277" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E277" s="57" t="s">
-        <v>3013</v>
+        <v>3012</v>
       </c>
       <c r="F277" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.35">
@@ -24238,14 +24244,14 @@
       <c r="C278" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D278" s="56" t="s">
-        <v>2930</v>
+      <c r="D278" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E278" s="57" t="s">
-        <v>3014</v>
+        <v>3013</v>
       </c>
       <c r="F278" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="279" spans="1:10" x14ac:dyDescent="0.35">
@@ -24258,14 +24264,14 @@
       <c r="C279" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D279" s="56" t="s">
-        <v>2930</v>
+      <c r="D279" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E279" s="57" t="s">
-        <v>3016</v>
+        <v>3015</v>
       </c>
       <c r="F279" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.35">
@@ -24278,14 +24284,14 @@
       <c r="C280" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D280" s="56" t="s">
-        <v>2930</v>
+      <c r="D280" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E280" s="57" t="s">
-        <v>3017</v>
+        <v>3016</v>
       </c>
       <c r="F280" t="s">
-        <v>2932</v>
+        <v>2931</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.35">
@@ -24298,14 +24304,14 @@
       <c r="C281" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D281" s="56" t="s">
-        <v>2930</v>
+      <c r="D281" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E281" s="57" t="s">
-        <v>3011</v>
+        <v>3010</v>
       </c>
       <c r="F281" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.35">
@@ -24318,14 +24324,14 @@
       <c r="C282" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D282" s="56" t="s">
-        <v>2930</v>
+      <c r="D282" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E282" s="57" t="s">
-        <v>3018</v>
+        <v>3017</v>
       </c>
       <c r="F282" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.35">
@@ -24338,14 +24344,14 @@
       <c r="C283" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D283" s="56" t="s">
-        <v>2930</v>
+      <c r="D283" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E283" s="57" t="s">
-        <v>3019</v>
+        <v>3018</v>
       </c>
       <c r="F283" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.35">
@@ -24358,14 +24364,14 @@
       <c r="C284" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D284" s="56" t="s">
-        <v>2930</v>
+      <c r="D284" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E284" s="57" t="s">
-        <v>3010</v>
+        <v>3009</v>
       </c>
       <c r="F284" t="s">
-        <v>2940</v>
+        <v>2939</v>
       </c>
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.35">
@@ -24378,14 +24384,14 @@
       <c r="C285" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D285" s="56" t="s">
-        <v>2930</v>
+      <c r="D285" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E285" s="57" t="s">
-        <v>3009</v>
+        <v>3008</v>
       </c>
       <c r="F285" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.35">
@@ -24398,14 +24404,14 @@
       <c r="C286" s="56" t="s">
         <v>2002</v>
       </c>
-      <c r="D286" s="56" t="s">
-        <v>2930</v>
+      <c r="D286" s="55" t="s">
+        <v>2929</v>
       </c>
       <c r="E286" s="57" t="s">
-        <v>3008</v>
+        <v>3007</v>
       </c>
       <c r="F286" t="s">
-        <v>2942</v>
+        <v>2941</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.35">
@@ -27907,7 +27913,7 @@
     </row>
     <row r="646" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A646" s="16" t="s">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="E646" t="s">
         <v>1943</v>
@@ -27915,7 +27921,7 @@
     </row>
     <row r="647" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A647" s="16" t="s">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="E647" t="s">
         <v>1945</v>
@@ -27923,7 +27929,7 @@
     </row>
     <row r="648" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A648" s="16" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="E648" t="s">
         <v>1947</v>
@@ -27933,7 +27939,7 @@
     </row>
     <row r="649" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A649" s="16" t="s">
-        <v>2984</v>
+        <v>2983</v>
       </c>
       <c r="E649" t="s">
         <v>1949</v>
@@ -27943,7 +27949,7 @@
     </row>
     <row r="650" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A650" s="16" t="s">
-        <v>2985</v>
+        <v>2984</v>
       </c>
       <c r="E650" t="s">
         <v>1951</v>
@@ -27953,7 +27959,7 @@
     </row>
     <row r="651" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A651" s="16" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="E651" t="s">
         <v>1953</v>
@@ -27963,7 +27969,7 @@
     </row>
     <row r="652" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A652" s="16" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="E652" t="s">
         <v>1955</v>
@@ -27973,7 +27979,7 @@
     </row>
     <row r="653" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A653" s="16" t="s">
-        <v>2988</v>
+        <v>2987</v>
       </c>
       <c r="E653" t="s">
         <v>1957</v>
@@ -27989,7 +27995,7 @@
     </row>
     <row r="654" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A654" s="16" t="s">
-        <v>2989</v>
+        <v>2988</v>
       </c>
       <c r="E654" t="s">
         <v>2832</v>
@@ -28002,7 +28008,7 @@
     </row>
     <row r="655" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A655" s="16" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="E655" t="s">
         <v>1959</v>
@@ -28015,7 +28021,7 @@
     </row>
     <row r="656" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A656" s="16" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="E656" t="s">
         <v>1961</v>
@@ -28025,7 +28031,7 @@
     </row>
     <row r="657" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A657" s="16" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="E657" t="s">
         <v>1963</v>
@@ -28047,25 +28053,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K107"/>
+  <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6328125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="10.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.1796875" customWidth="1"/>
-    <col min="8" max="8" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.26953125" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" customWidth="1"/>
+    <col min="4" max="6" width="10.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1796875" customWidth="1"/>
+    <col min="9" max="9" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.26953125" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="15" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="15" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -28082,17 +28088,20 @@
         <v>2197</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>3019</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>2491</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>527</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>528</v>
       </c>
-      <c r="I1" s="21"/>
-    </row>
-    <row r="2" spans="1:11" s="14" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" s="14" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>14</v>
       </c>
@@ -28104,16 +28113,17 @@
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="41"/>
+      <c r="G2" s="41" t="s">
         <v>531</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="H2" s="42" t="s">
         <v>530</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I2" s="42"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -28123,15 +28133,15 @@
       <c r="C3" s="41" t="s">
         <v>2314</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="H3" s="43" t="s">
         <v>534</v>
       </c>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -28147,20 +28157,20 @@
       <c r="E4" s="1" t="s">
         <v>2198</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="H4" s="25" t="s">
         <v>2316</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="25" t="s">
         <v>2355</v>
       </c>
-      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -28170,15 +28180,15 @@
       <c r="C5" s="41" t="s">
         <v>2318</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="H5" s="25" t="s">
         <v>2320</v>
       </c>
-      <c r="H5" s="25"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -28188,15 +28198,15 @@
       <c r="C6" s="41" t="s">
         <v>2321</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="H6" s="25" t="s">
         <v>538</v>
       </c>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -28206,17 +28216,17 @@
       <c r="C7" s="42" t="s">
         <v>2322</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="H7" s="25" t="s">
         <v>2323</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="I7" s="25" t="s">
         <v>2325</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -28226,17 +28236,17 @@
       <c r="C8" s="42" t="s">
         <v>2322</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>2324</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="H8" s="25" t="s">
         <v>2363</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="I8" s="25" t="s">
         <v>2326</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>517</v>
       </c>
@@ -28246,17 +28256,17 @@
       <c r="C9" s="42" t="s">
         <v>2327</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>2328</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="I9" s="25" t="s">
         <v>2329</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
@@ -28269,17 +28279,17 @@
       <c r="E10" s="1" t="s">
         <v>2198</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="H10" s="25" t="s">
         <v>2320</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="I10" s="25" t="s">
         <v>2356</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>539</v>
       </c>
@@ -28295,17 +28305,17 @@
       <c r="E11" s="1" t="s">
         <v>2198</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>2337</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="H11" s="25" t="s">
         <v>2364</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="I11" s="25" t="s">
         <v>2357</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>540</v>
       </c>
@@ -28315,15 +28325,15 @@
       <c r="C12" s="41" t="s">
         <v>2336</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="H12" s="25" t="s">
         <v>2338</v>
       </c>
-      <c r="H12" s="25"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>541</v>
       </c>
@@ -28333,15 +28343,15 @@
       <c r="C13" s="41" t="s">
         <v>2318</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>2337</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="H13" s="25" t="s">
         <v>2365</v>
       </c>
-      <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>542</v>
       </c>
@@ -28351,15 +28361,15 @@
       <c r="C14" s="41" t="s">
         <v>2314</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>2324</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="H14" s="25" t="s">
         <v>2389</v>
       </c>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>543</v>
       </c>
@@ -28369,15 +28379,15 @@
       <c r="C15" s="41" t="s">
         <v>2314</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>2761</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="H15" s="25" t="s">
         <v>2762</v>
       </c>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>544</v>
       </c>
@@ -28387,15 +28397,15 @@
       <c r="C16" s="41" t="s">
         <v>2314</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>2361</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="H16" s="25" t="s">
         <v>2366</v>
       </c>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>545</v>
       </c>
@@ -28405,15 +28415,15 @@
       <c r="C17" s="41" t="s">
         <v>2314</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>2362</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="H17" s="25" t="s">
         <v>2367</v>
       </c>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>546</v>
       </c>
@@ -28429,17 +28439,17 @@
       <c r="E18" s="1" t="s">
         <v>2198</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>2370</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="H18" s="25" t="s">
         <v>2372</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="I18" s="25" t="s">
         <v>2371</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>547</v>
       </c>
@@ -28449,14 +28459,14 @@
       <c r="C19" s="1" t="s">
         <v>2314</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="G19" s="25" t="s">
         <v>2373</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="H19" s="25" t="s">
         <v>2374</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>548</v>
       </c>
@@ -28466,14 +28476,14 @@
       <c r="C20" s="1" t="s">
         <v>2313</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>2324</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="H20" s="25" t="s">
         <v>2385</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>549</v>
       </c>
@@ -28483,14 +28493,14 @@
       <c r="C21" s="1" t="s">
         <v>2314</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>2337</v>
       </c>
-      <c r="G21" s="25" t="s">
+      <c r="H21" s="25" t="s">
         <v>2437</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>550</v>
       </c>
@@ -28500,14 +28510,14 @@
       <c r="C22" s="1" t="s">
         <v>2314</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>2481</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="H22" s="25" t="s">
         <v>2482</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>551</v>
       </c>
@@ -28517,11 +28527,11 @@
       <c r="C23" s="1" t="s">
         <v>2490</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>552</v>
       </c>
@@ -28537,17 +28547,17 @@
       <c r="E24" s="1" t="s">
         <v>2533</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>2324</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="H24" s="25" t="s">
         <v>2534</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="I24" s="25" t="s">
         <v>2539</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>553</v>
       </c>
@@ -28563,17 +28573,17 @@
       <c r="E25" s="1" t="s">
         <v>2533</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>2324</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="H25" s="25" t="s">
         <v>2540</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="I25" s="25" t="s">
         <v>2541</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>554</v>
       </c>
@@ -28589,17 +28599,17 @@
       <c r="E26" s="1" t="s">
         <v>2533</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>2324</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="H26" s="25" t="s">
         <v>2552</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="I26" s="25" t="s">
         <v>2553</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>555</v>
       </c>
@@ -28609,14 +28619,14 @@
       <c r="C27" s="1" t="s">
         <v>2660</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G27" s="25" t="s">
+      <c r="H27" s="25" t="s">
         <v>2661</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>556</v>
       </c>
@@ -28626,14 +28636,14 @@
       <c r="C28" s="1" t="s">
         <v>2673</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="H28" s="25" t="s">
         <v>2674</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>557</v>
       </c>
@@ -28643,14 +28653,14 @@
       <c r="C29" s="1" t="s">
         <v>2684</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G29" s="25" t="s">
+      <c r="H29" s="25" t="s">
         <v>2685</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>558</v>
       </c>
@@ -28660,14 +28670,14 @@
       <c r="C30" s="1" t="s">
         <v>2686</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G30" s="25" t="s">
+      <c r="H30" s="25" t="s">
         <v>2687</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>559</v>
       </c>
@@ -28677,14 +28687,14 @@
       <c r="C31" s="25" t="s">
         <v>2688</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="G31" s="25" t="s">
+      <c r="H31" s="25" t="s">
         <v>2689</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>560</v>
       </c>
@@ -28694,14 +28704,14 @@
       <c r="C32" s="1" t="s">
         <v>2314</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>2370</v>
       </c>
-      <c r="G32" s="25" t="s">
+      <c r="H32" s="25" t="s">
         <v>2694</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>561</v>
       </c>
@@ -28711,14 +28721,14 @@
       <c r="C33" s="1" t="s">
         <v>2759</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="H33" s="25" t="s">
+      <c r="I33" s="25" t="s">
         <v>2760</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>562</v>
       </c>
@@ -28728,20 +28738,26 @@
       <c r="C34" s="1" t="s">
         <v>2313</v>
       </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>2198</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="1">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>2337</v>
       </c>
-      <c r="G34" s="25" t="s">
+      <c r="H34" s="25" t="s">
         <v>2895</v>
       </c>
-      <c r="H34" s="25" t="s">
-        <v>2918</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34" s="25" t="s">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>563</v>
       </c>
@@ -28757,17 +28773,17 @@
       <c r="E35" s="1" t="s">
         <v>2198</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>2324</v>
       </c>
-      <c r="G35" s="25" t="s">
+      <c r="H35" s="25" t="s">
+        <v>2922</v>
+      </c>
+      <c r="I35" s="25" t="s">
         <v>2923</v>
       </c>
-      <c r="H35" s="25" t="s">
-        <v>2924</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>564</v>
       </c>
@@ -28777,69 +28793,93 @@
       <c r="C36" s="1" t="s">
         <v>2314</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
+        <v>3005</v>
+      </c>
+      <c r="H36" s="25" t="s">
         <v>3006</v>
       </c>
-      <c r="G36" s="25" t="s">
-        <v>3007</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B37" s="41" t="s">
+        <v>529</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>2313</v>
+      </c>
+      <c r="D37" s="41">
+        <v>1</v>
+      </c>
+      <c r="E37" s="41" t="s">
+        <v>2198</v>
+      </c>
+      <c r="F37" s="41">
+        <v>3</v>
+      </c>
+      <c r="G37" s="41" t="s">
+        <v>531</v>
+      </c>
+      <c r="H37" s="42" t="s">
+        <v>530</v>
+      </c>
+      <c r="I37" s="42" t="s">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>576</v>
       </c>
@@ -29333,10 +29373,10 @@
         <v>639</v>
       </c>
       <c r="C7" s="32" t="s">
+        <v>2927</v>
+      </c>
+      <c r="D7" t="s">
         <v>2928</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2929</v>
       </c>
       <c r="E7" t="s">
         <v>2195</v>
@@ -30076,7 +30116,7 @@
         <v>2199</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>2921</v>
+        <v>2920</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>2201</v>
@@ -30134,7 +30174,7 @@
         <v>2199</v>
       </c>
       <c r="C35" s="46" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>2201</v>
@@ -35673,10 +35713,10 @@
         <v>639</v>
       </c>
       <c r="C226" s="57" t="s">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="D226" s="24" t="s">
-        <v>2955</v>
+        <v>2954</v>
       </c>
       <c r="E226" t="s">
         <v>2157</v>
@@ -35688,7 +35728,7 @@
         <v>2021</v>
       </c>
       <c r="I226" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J226" t="s">
         <v>643</v>
@@ -35702,10 +35742,10 @@
         <v>639</v>
       </c>
       <c r="C227" s="57" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="D227" s="24" t="s">
-        <v>2956</v>
+        <v>2955</v>
       </c>
       <c r="E227" t="s">
         <v>2157</v>
@@ -35717,7 +35757,7 @@
         <v>2021</v>
       </c>
       <c r="I227" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J227" t="s">
         <v>643</v>
@@ -35731,10 +35771,10 @@
         <v>639</v>
       </c>
       <c r="C228" s="57" t="s">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="D228" s="24" t="s">
-        <v>2957</v>
+        <v>2956</v>
       </c>
       <c r="E228" t="s">
         <v>2157</v>
@@ -35746,7 +35786,7 @@
         <v>2021</v>
       </c>
       <c r="I228" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J228" t="s">
         <v>643</v>
@@ -35760,10 +35800,10 @@
         <v>639</v>
       </c>
       <c r="C229" s="57" t="s">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="D229" s="24" t="s">
-        <v>2958</v>
+        <v>2957</v>
       </c>
       <c r="E229" t="s">
         <v>2157</v>
@@ -35775,7 +35815,7 @@
         <v>2021</v>
       </c>
       <c r="I229" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J229" t="s">
         <v>643</v>
@@ -35789,10 +35829,10 @@
         <v>639</v>
       </c>
       <c r="C230" s="57" t="s">
-        <v>2947</v>
+        <v>2946</v>
       </c>
       <c r="D230" s="24" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="E230" t="s">
         <v>2157</v>
@@ -35804,7 +35844,7 @@
         <v>2021</v>
       </c>
       <c r="I230" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J230" t="s">
         <v>643</v>
@@ -35818,10 +35858,10 @@
         <v>639</v>
       </c>
       <c r="C231" s="57" t="s">
-        <v>2948</v>
+        <v>2947</v>
       </c>
       <c r="D231" s="24" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
       <c r="E231" t="s">
         <v>2157</v>
@@ -35833,7 +35873,7 @@
         <v>2021</v>
       </c>
       <c r="I231" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J231" t="s">
         <v>643</v>
@@ -35847,10 +35887,10 @@
         <v>639</v>
       </c>
       <c r="C232" s="57" t="s">
-        <v>2949</v>
+        <v>2948</v>
       </c>
       <c r="D232" s="24" t="s">
-        <v>2961</v>
+        <v>2960</v>
       </c>
       <c r="E232" t="s">
         <v>2157</v>
@@ -35862,7 +35902,7 @@
         <v>2021</v>
       </c>
       <c r="I232" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J232" t="s">
         <v>643</v>
@@ -35876,10 +35916,10 @@
         <v>639</v>
       </c>
       <c r="C233" s="57" t="s">
-        <v>2950</v>
+        <v>2949</v>
       </c>
       <c r="D233" s="24" t="s">
-        <v>2962</v>
+        <v>2961</v>
       </c>
       <c r="E233" t="s">
         <v>2157</v>
@@ -35891,7 +35931,7 @@
         <v>2021</v>
       </c>
       <c r="I233" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J233" t="s">
         <v>643</v>
@@ -35899,16 +35939,16 @@
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>639</v>
       </c>
       <c r="C234" s="57" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="D234" s="24" t="s">
-        <v>2963</v>
+        <v>2962</v>
       </c>
       <c r="E234" t="s">
         <v>2157</v>
@@ -35920,7 +35960,7 @@
         <v>2021</v>
       </c>
       <c r="I234" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J234" t="s">
         <v>643</v>
@@ -35928,16 +35968,16 @@
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>639</v>
       </c>
       <c r="C235" s="57" t="s">
-        <v>2952</v>
+        <v>2951</v>
       </c>
       <c r="D235" s="24" t="s">
-        <v>2964</v>
+        <v>2963</v>
       </c>
       <c r="E235" t="s">
         <v>2157</v>
@@ -35949,7 +35989,7 @@
         <v>2021</v>
       </c>
       <c r="I235" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J235" t="s">
         <v>643</v>
@@ -35957,16 +35997,16 @@
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>639</v>
       </c>
       <c r="C236" s="57" t="s">
-        <v>2953</v>
+        <v>2952</v>
       </c>
       <c r="D236" s="24" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="E236" t="s">
         <v>2157</v>
@@ -35978,7 +36018,7 @@
         <v>2021</v>
       </c>
       <c r="I236" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J236" t="s">
         <v>643</v>
@@ -35986,16 +36026,16 @@
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>639</v>
       </c>
       <c r="C237" s="57" t="s">
-        <v>2954</v>
+        <v>2953</v>
       </c>
       <c r="D237" s="24" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="E237" t="s">
         <v>2157</v>
@@ -36007,7 +36047,7 @@
         <v>2021</v>
       </c>
       <c r="I237" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="J237" t="s">
         <v>643</v>
@@ -36022,7 +36062,7 @@
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>639</v>
@@ -36051,7 +36091,7 @@
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>639</v>
@@ -36080,7 +36120,7 @@
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>639</v>
@@ -36109,7 +36149,7 @@
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>639</v>
@@ -36138,7 +36178,7 @@
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>639</v>
@@ -36167,7 +36207,7 @@
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
-        <v>2977</v>
+        <v>2976</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>2158</v>
@@ -36193,7 +36233,7 @@
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>2158</v>
@@ -36219,7 +36259,7 @@
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>2158</v>
@@ -36245,7 +36285,7 @@
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>2158</v>

</xml_diff>